<commit_message>
Added calcium and b12 to Zambia and Uganda and updated output
</commit_message>
<xml_diff>
--- a/output/b12_SPADE_uganda_h/3_excel_tables/spade_uganda_h_b12.xlsx
+++ b/output/b12_SPADE_uganda_h/3_excel_tables/spade_uganda_h_b12.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="179">
   <si>
     <t xml:space="preserve"/>
   </si>
@@ -208,13 +208,13 @@
     <t xml:space="preserve">Start_time</t>
   </si>
   <si>
-    <t xml:space="preserve">Fri Nov 13 10:06:53 2020</t>
+    <t xml:space="preserve">Thu Nov 19 15:23:38 2020</t>
   </si>
   <si>
     <t xml:space="preserve">End_time</t>
   </si>
   <si>
-    <t xml:space="preserve">Fri Nov 13 10:06:59 2020</t>
+    <t xml:space="preserve">Thu Nov 19 15:23:45 2020</t>
   </si>
   <si>
     <t xml:space="preserve">sheet_description</t>
@@ -388,7 +388,7 @@
     <t xml:space="preserve">here</t>
   </si>
   <si>
-    <t xml:space="preserve">0.1</t>
+    <t xml:space="preserve">1.0.0</t>
   </si>
   <si>
     <t xml:space="preserve">4.0.079</t>
@@ -484,7 +484,7 @@
     <t xml:space="preserve">magrittr</t>
   </si>
   <si>
-    <t xml:space="preserve">1.5</t>
+    <t xml:space="preserve">2.0.1</t>
   </si>
   <si>
     <t xml:space="preserve">statmod</t>
@@ -523,7 +523,7 @@
     <t xml:space="preserve">rprojroot</t>
   </si>
   <si>
-    <t xml:space="preserve">1.3-2</t>
+    <t xml:space="preserve">2.0.2</t>
   </si>
   <si>
     <t xml:space="preserve">zip</t>
@@ -545,12 +545,6 @@
   </si>
   <si>
     <t xml:space="preserve">compiler</t>
-  </si>
-  <si>
-    <t xml:space="preserve">backports</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.1.10</t>
   </si>
   <si>
     <t xml:space="preserve">boot</t>
@@ -1924,12 +1918,6 @@
       <c r="G16" t="s">
         <v>151</v>
       </c>
-      <c r="I16" t="s">
-        <v>179</v>
-      </c>
-      <c r="J16" t="s">
-        <v>180</v>
-      </c>
     </row>
     <row r="17">
       <c r="A17" t="s">

</xml_diff>